<commit_message>
removed a weird annotation
</commit_message>
<xml_diff>
--- a/data/annotated_scripts.xlsx
+++ b/data/annotated_scripts.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Main script" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Main script'!$E$8:$E$151</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="Z_E7F284B7_B5F7_4D04_B2BD_CA5521DD5FA3_.wvu.FilterData" vbProcedure="false">'Main script'!$E$1:$E$157</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Main script'!$E$8:$E$150</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="Z_E7F284B7_B5F7_4D04_B2BD_CA5521DD5FA3_.wvu.FilterData" vbProcedure="false">'Main script'!$E$1:$E$156</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="300">
   <si>
     <t xml:space="preserve">Grace Dialogflow Script - 09/08/2023</t>
   </si>
@@ -4922,187 +4922,6 @@
   </si>
   <si>
     <t xml:space="preserve">Q5.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">喺哩間房入面，如果有醫生或者護士，你可唔可以指出邊個係醫生，邊個係護士？</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In this room, if there are any nurses or doctors, would you be able to tell who is a nurse, and who is a doctor?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hai2 lei1 gaan1 fong2 jap6 min6, jyu4 gwo2 jau5 ji1 saang1 waak6 ze2 wu6 si6, nei5 ho2 m4 ho2 ji5 zi2 ceot1 bin1 go3 hai6 ji1 saang1, bin1 go3 hai6 wu6 si6?</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">喺哩間房入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;phoneme alphabet="x-amazon-jyutping" ph="min6"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">面</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/phoneme&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">，如果有醫生或者護</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;phoneme alphabet="x-amazon-jyutping" ph="si6"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">士</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/phoneme&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">，你可唔可以指出邊個係醫</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;phoneme alphabet="x-amazon-jyutping" ph="hai2 lei1 gaan1 fong2 jap6 min6, jyu4 gwo2 jau5 ji1 saang1 waak6 ze2 wu6 si6, nei5 ho2 m4 ho2 ji5 zi2 ceot1 bin1 go3 hai6 ji1 saang1"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">生</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/phoneme&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">，邊個係護</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;phoneme alphabet="x-amazon-jyutping" ph="si6"&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">士</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;/phoneme&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">？</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Intent 1: 
@@ -9613,7 +9432,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -9706,12 +9525,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="5">
@@ -10110,7 +9923,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10206,7 +10019,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+      <selection pane="topLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11279,157 +11092,143 @@
       </c>
       <c r="F76" s="12"/>
     </row>
-    <row r="77" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B77" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="D77" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E77" s="22"/>
+    </row>
+    <row r="78" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="13"/>
+      <c r="B78" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C77" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="D77" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="E77" s="42" t="s">
-        <v>166</v>
-      </c>
-      <c r="F77" s="18" t="s">
+      <c r="C78" s="24" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="13" t="s">
+      <c r="D78" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B78" s="19" t="s">
+      <c r="E78" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="D78" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="E78" s="22"/>
-    </row>
-    <row r="79" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="13"/>
-      <c r="B79" s="23" t="s">
+      <c r="C79" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E79" s="22"/>
+    </row>
+    <row r="80" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="13"/>
+      <c r="B80" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="D79" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="E79" s="26" t="s">
+      <c r="C80" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="F79" s="24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="13" t="s">
+      <c r="D80" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="B80" s="19" t="s">
+      <c r="E80" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="B81" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C80" s="20" t="s">
+      <c r="C81" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D81" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E81" s="22"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="13"/>
+      <c r="B82" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E82" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="D80" s="28" t="s">
+      <c r="F82" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="E80" s="22"/>
-    </row>
-    <row r="81" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="13"/>
-      <c r="B81" s="23" t="s">
+    </row>
+    <row r="83" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E83" s="27"/>
+    </row>
+    <row r="84" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="13"/>
+      <c r="B84" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="D81" s="29" t="s">
+      <c r="C84" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="E81" s="26" t="s">
+      <c r="D84" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="F81" s="12" t="s">
+      <c r="E84" s="26" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="13" t="s">
+      <c r="F84" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="B82" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C82" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D82" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E82" s="22"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="13"/>
-      <c r="B83" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C83" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="D83" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="E83" s="26" t="s">
-        <v>179</v>
-      </c>
-      <c r="F83" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B84" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D84" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E84" s="27"/>
-    </row>
-    <row r="85" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="13"/>
-      <c r="B85" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="D85" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="E85" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="F85" s="18" t="s">
-        <v>185</v>
-      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="35"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="35"/>
@@ -11437,146 +11236,146 @@
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="35"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="9" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B87" s="9"/>
+      <c r="C87" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="12"/>
+    </row>
+    <row r="88" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E88" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="F88" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="B88" s="9"/>
-      <c r="C88" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E88" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F88" s="12"/>
-    </row>
-    <row r="89" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="D89" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E89" s="22"/>
+    </row>
+    <row r="90" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="13"/>
+      <c r="B90" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C89" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="D89" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="E89" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="F89" s="18" t="s">
+      <c r="C90" s="24" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="90" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="13" t="s">
+      <c r="D90" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="B90" s="19" t="s">
+      <c r="E90" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B91" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C90" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D90" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="E90" s="22"/>
-    </row>
-    <row r="91" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="13"/>
-      <c r="B91" s="23" t="s">
+      <c r="C91" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D91" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E91" s="22"/>
+    </row>
+    <row r="92" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="13"/>
+      <c r="B92" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C91" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D91" s="43" t="s">
+      <c r="C92" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="E91" s="26" t="s">
+      <c r="D92" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="E92" s="26" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="13" t="s">
+      <c r="F92" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B92" s="19" t="s">
+    </row>
+    <row r="93" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C92" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D92" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E92" s="22"/>
-    </row>
-    <row r="93" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="13"/>
-      <c r="B93" s="23" t="s">
+      <c r="C93" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D93" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E93" s="27"/>
+    </row>
+    <row r="94" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="13"/>
+      <c r="B94" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C93" s="24" t="s">
+      <c r="C94" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="D93" s="29" t="s">
+      <c r="D94" s="29" t="s">
         <v>200</v>
       </c>
-      <c r="E93" s="26" t="s">
+      <c r="E94" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="F93" s="18" t="s">
+      <c r="F94" s="18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B94" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C94" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D94" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E94" s="27"/>
-    </row>
-    <row r="95" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="13"/>
-      <c r="B95" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C95" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="D95" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="E95" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="F95" s="18" t="s">
-        <v>206</v>
-      </c>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="35"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="35"/>
@@ -11602,146 +11401,146 @@
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="35"/>
-      <c r="B100" s="7"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="9" t="s">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B100" s="9"/>
+      <c r="C100" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F100" s="12"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="38" t="s">
+        <v>204</v>
+      </c>
+      <c r="D101" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="E101" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F101" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E101" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F101" s="12"/>
-    </row>
-    <row r="102" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="102" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B102" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B102" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C102" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="D102" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="E102" s="22"/>
+    </row>
+    <row r="103" customFormat="false" ht="70.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="13"/>
+      <c r="B103" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C102" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="D102" s="39" t="s">
-        <v>209</v>
-      </c>
-      <c r="E102" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="F102" s="18" t="s">
+      <c r="C103" s="24" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="103" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="13" t="s">
+      <c r="D103" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="E103" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A104" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C103" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="D103" s="41" t="s">
-        <v>214</v>
-      </c>
-      <c r="E103" s="22"/>
-    </row>
-    <row r="104" customFormat="false" ht="70.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="13"/>
-      <c r="B104" s="23" t="s">
+      <c r="C104" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D104" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E104" s="22"/>
+    </row>
+    <row r="105" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A105" s="13"/>
+      <c r="B105" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C104" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="D104" s="29" t="s">
+      <c r="C105" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="E104" s="26" t="s">
+      <c r="D105" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="F104" s="18" t="s">
+      <c r="E105" s="26" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="13" t="s">
+      <c r="F105" s="18" t="s">
         <v>219</v>
       </c>
-      <c r="B105" s="19" t="s">
+    </row>
+    <row r="106" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A106" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B106" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C105" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D105" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="E105" s="22"/>
-    </row>
-    <row r="106" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="13"/>
-      <c r="B106" s="23" t="s">
+      <c r="C106" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E106" s="27"/>
+    </row>
+    <row r="107" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="13"/>
+      <c r="B107" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C106" s="24" t="s">
+      <c r="C107" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="D106" s="45" t="s">
+      <c r="D107" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="E106" s="26" t="s">
+      <c r="E107" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="F106" s="18" t="s">
+      <c r="F107" s="18" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B107" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C107" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D107" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E107" s="27"/>
-    </row>
-    <row r="108" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="13"/>
-      <c r="B108" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C108" s="24" t="s">
-        <v>224</v>
-      </c>
-      <c r="D108" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="E108" s="26" t="s">
-        <v>226</v>
-      </c>
-      <c r="F108" s="18" t="s">
-        <v>227</v>
-      </c>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="35"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="35"/>
@@ -11755,179 +11554,179 @@
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="35"/>
-      <c r="B111" s="7"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="9" t="s">
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A111" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B111" s="9"/>
+      <c r="C111" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F111" s="12"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C112" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="D112" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="E112" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="F112" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="B112" s="9"/>
-      <c r="C112" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E112" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F112" s="12"/>
-    </row>
-    <row r="113" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="113" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B113" s="40" t="s">
+        <v>229</v>
+      </c>
+      <c r="B113" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="D113" s="41" t="s">
+        <v>231</v>
+      </c>
+      <c r="E113" s="22"/>
+    </row>
+    <row r="114" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="13"/>
+      <c r="B114" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C113" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="D113" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="E113" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="F113" s="18" t="s">
+      <c r="C114" s="24" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="114" customFormat="false" ht="19.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="13" t="s">
+      <c r="D114" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="B114" s="19" t="s">
+      <c r="E114" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="F114" s="18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B115" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C114" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="D114" s="41" t="s">
-        <v>235</v>
-      </c>
-      <c r="E114" s="22"/>
-    </row>
-    <row r="115" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="13"/>
-      <c r="B115" s="23" t="s">
+      <c r="C115" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="D115" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="E115" s="22"/>
+    </row>
+    <row r="116" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="13"/>
+      <c r="B116" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C115" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="D115" s="45" t="s">
-        <v>237</v>
-      </c>
-      <c r="E115" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="F115" s="18" t="s">
+      <c r="C116" s="46" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="13" t="s">
+      <c r="D116" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="B116" s="19" t="s">
+      <c r="E116" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="F116" s="12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B117" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C116" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="D116" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="E116" s="22"/>
-    </row>
-    <row r="117" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="13"/>
-      <c r="B117" s="23" t="s">
+      <c r="C117" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D117" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E117" s="22"/>
+    </row>
+    <row r="118" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="13"/>
+      <c r="B118" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C117" s="46" t="s">
-        <v>243</v>
-      </c>
-      <c r="D117" s="47" t="s">
+      <c r="C118" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="E117" s="26" t="s">
+      <c r="D118" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="F117" s="12" t="s">
+      <c r="E118" s="26" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="118" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="13" t="s">
+      <c r="F118" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="B118" s="19" t="s">
+    </row>
+    <row r="119" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A119" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B119" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C118" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D118" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E118" s="22"/>
-    </row>
-    <row r="119" customFormat="false" ht="28.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="13"/>
-      <c r="B119" s="23" t="s">
+      <c r="C119" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D119" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E119" s="27"/>
+    </row>
+    <row r="120" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="13"/>
+      <c r="B120" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C119" s="24" t="s">
+      <c r="C120" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="D119" s="29" t="s">
+      <c r="D120" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="E119" s="26" t="s">
+      <c r="E120" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="F119" s="12" t="s">
+      <c r="F120" s="18" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B120" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C120" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D120" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E120" s="27"/>
-    </row>
-    <row r="121" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="13"/>
-      <c r="B121" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C121" s="24" t="s">
-        <v>252</v>
-      </c>
-      <c r="D121" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="E121" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="F121" s="18" t="s">
-        <v>255</v>
-      </c>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="35"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="8"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="35"/>
@@ -11935,105 +11734,105 @@
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="35"/>
-      <c r="B123" s="7"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="9" t="s">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A123" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B123" s="9"/>
+      <c r="C123" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D123" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F123" s="12"/>
+    </row>
+    <row r="124" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A124" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="B124" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="D124" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="E124" s="22"/>
+    </row>
+    <row r="125" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A125" s="13"/>
+      <c r="B125" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D125" s="49" t="s">
         <v>256</v>
       </c>
-      <c r="B124" s="9"/>
-      <c r="C124" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D124" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E124" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F124" s="12"/>
-    </row>
-    <row r="125" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="13" t="s">
+      <c r="E125" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="B125" s="19" t="s">
+      <c r="F125" s="24" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A126" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="B126" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C125" s="48" t="s">
-        <v>258</v>
-      </c>
-      <c r="D125" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="E125" s="22"/>
-    </row>
-    <row r="126" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="13"/>
-      <c r="B126" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C126" s="24" t="s">
+      <c r="C126" s="48" t="s">
         <v>259</v>
       </c>
-      <c r="D126" s="49" t="s">
+      <c r="D126" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="E126" s="22"/>
+    </row>
+    <row r="127" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A127" s="13" t="s">
         <v>260</v>
-      </c>
-      <c r="E126" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="F126" s="24" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="13" t="s">
-        <v>262</v>
       </c>
       <c r="B127" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C127" s="48" t="s">
-        <v>263</v>
+      <c r="C127" s="20" t="s">
+        <v>261</v>
       </c>
       <c r="D127" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E127" s="22"/>
     </row>
-    <row r="128" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="13" t="s">
-        <v>264</v>
+        <v>34</v>
       </c>
       <c r="B128" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>265</v>
+        <v>35</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>266</v>
-      </c>
-      <c r="E128" s="22"/>
-    </row>
-    <row r="129" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B129" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C129" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D129" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E129" s="27"/>
+      <c r="E128" s="27"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="35"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="8"/>
+      <c r="D129" s="8"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="35"/>
@@ -12059,179 +11858,179 @@
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="35"/>
-      <c r="B134" s="7"/>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="9" t="s">
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A134" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="B134" s="9"/>
+      <c r="C134" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D134" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E134" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F134" s="12"/>
+    </row>
+    <row r="135" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="D135" s="39" t="s">
+        <v>265</v>
+      </c>
+      <c r="E135" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="F135" s="18" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="9"/>
-      <c r="C135" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D135" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E135" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F135" s="12"/>
-    </row>
-    <row r="136" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="136" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B136" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="B136" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D136" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E136" s="22"/>
+    </row>
+    <row r="137" customFormat="false" ht="42.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="13"/>
+      <c r="B137" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C136" s="38" t="s">
-        <v>268</v>
-      </c>
-      <c r="D136" s="39" t="s">
+      <c r="C137" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="E136" s="17" t="s">
+      <c r="D137" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="F136" s="18" t="s">
+      <c r="E137" s="26" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="137" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="13" t="s">
+      <c r="F137" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="B137" s="19" t="s">
+    </row>
+    <row r="138" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A138" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B138" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C137" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D137" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E137" s="22"/>
-    </row>
-    <row r="138" customFormat="false" ht="42.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="13"/>
-      <c r="B138" s="23" t="s">
+      <c r="C138" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D138" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E138" s="22"/>
+    </row>
+    <row r="139" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="13"/>
+      <c r="B139" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C138" s="24" t="s">
-        <v>273</v>
-      </c>
-      <c r="D138" s="29" t="s">
+      <c r="C139" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="E138" s="26" t="s">
+      <c r="D139" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="F138" s="18" t="s">
+      <c r="E139" s="26" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="139" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="13" t="s">
+      <c r="F139" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B139" s="19" t="s">
+    </row>
+    <row r="140" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A140" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C139" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="D139" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E139" s="22"/>
-    </row>
-    <row r="140" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="13"/>
-      <c r="B140" s="23" t="s">
+      <c r="C140" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="D140" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="E140" s="22"/>
+    </row>
+    <row r="141" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="13"/>
+      <c r="B141" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C140" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="D140" s="29" t="s">
-        <v>279</v>
-      </c>
-      <c r="E140" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="F140" s="12" t="s">
+      <c r="C141" s="24" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="141" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="13" t="s">
+      <c r="D141" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="B141" s="19" t="s">
+      <c r="E141" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="F141" s="18" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A142" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B142" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C141" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="D141" s="28" t="s">
-        <v>284</v>
-      </c>
-      <c r="E141" s="22"/>
-    </row>
-    <row r="142" customFormat="false" ht="13.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="13"/>
-      <c r="B142" s="23" t="s">
+      <c r="C142" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D142" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E142" s="27"/>
+    </row>
+    <row r="143" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="13"/>
+      <c r="B143" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C142" s="24" t="s">
+      <c r="C143" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="D142" s="29" t="s">
+      <c r="D143" s="29" t="s">
         <v>286</v>
       </c>
-      <c r="E142" s="26" t="s">
+      <c r="E143" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="F142" s="18" t="s">
+      <c r="F143" s="18" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B143" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C143" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D143" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E143" s="27"/>
-    </row>
-    <row r="144" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="13"/>
-      <c r="B144" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C144" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="D144" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="E144" s="26" t="s">
-        <v>291</v>
-      </c>
-      <c r="F144" s="18" t="s">
-        <v>292</v>
-      </c>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="35"/>
+      <c r="B144" s="7"/>
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="35"/>
@@ -12239,81 +12038,80 @@
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="35"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="8"/>
-      <c r="D146" s="8"/>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="9" t="s">
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A146" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B146" s="9"/>
+      <c r="C146" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D146" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A147" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B147" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C147" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="D147" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="E147" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F147" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="B147" s="9"/>
-      <c r="C147" s="10" t="s">
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="35"/>
+      <c r="B148" s="7"/>
+      <c r="C148" s="8"/>
+      <c r="D148" s="8"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A149" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B149" s="9"/>
+      <c r="C149" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D147" s="10" t="s">
+      <c r="D149" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="B148" s="51" t="s">
+    <row r="150" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A150" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="B150" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="C148" s="52" t="s">
-        <v>294</v>
-      </c>
-      <c r="D148" s="53" t="s">
-        <v>295</v>
-      </c>
-      <c r="E148" s="12" t="s">
+      <c r="C150" s="55" t="s">
         <v>296</v>
       </c>
-      <c r="F148" s="18" t="s">
+      <c r="D150" s="56" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="35"/>
-      <c r="B149" s="7"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="9" t="s">
+      <c r="E150" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="B150" s="9"/>
-      <c r="C150" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D150" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="81" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="13" t="s">
+      <c r="F150" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="B151" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C151" s="55" t="s">
-        <v>300</v>
-      </c>
-      <c r="D151" s="56" t="s">
-        <v>301</v>
-      </c>
-      <c r="E151" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="F151" s="18" t="s">
-        <v>303</v>
-      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="2"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2"/>
@@ -12340,11 +12138,7 @@
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
     </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
-    </row>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -12362,7 +12156,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="E8:E151"/>
+  <autoFilter ref="E8:E150"/>
   <mergeCells count="53">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:A11"/>
@@ -12391,32 +12185,32 @@
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="A72:A73"/>
     <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A149:B149"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>